<commit_message>
added manual sheet download button, delete rows button, and added protection for overflowing sheet
</commit_message>
<xml_diff>
--- a/src/sheets/displaySheets/scouting.xlsx
+++ b/src/sheets/displaySheets/scouting.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,6 +426,9 @@
       <c r="C2" t="str">
         <v>3</v>
       </c>
+      <c r="D2" t="str">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -437,102 +440,13 @@
       <c r="C3" t="str">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2</v>
-      </c>
-      <c r="C4" t="str">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2</v>
-      </c>
-      <c r="C5" t="str">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2</v>
-      </c>
-      <c r="C6" t="str">
-        <v>3</v>
-      </c>
-      <c r="D6" t="str">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2</v>
-      </c>
-      <c r="C7" t="str">
-        <v>3</v>
-      </c>
-      <c r="D7" t="str">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <v>2</v>
-      </c>
-      <c r="C8" t="str">
-        <v>3</v>
-      </c>
-      <c r="D8" t="str">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>1</v>
-      </c>
-      <c r="B9" t="str">
-        <v>2</v>
-      </c>
-      <c r="C9" t="str">
-        <v>3</v>
-      </c>
-      <c r="D9" t="str">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <v>2</v>
-      </c>
-      <c r="C10" t="str">
-        <v>3</v>
-      </c>
-      <c r="D10" t="str">
+      <c r="D3" t="str">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added submiting to form template
</commit_message>
<xml_diff>
--- a/src/sheets/displaySheets/scouting.xlsx
+++ b/src/sheets/displaySheets/scouting.xlsx
@@ -397,56 +397,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>hello_column</v>
+        <v>matchNum</v>
       </c>
       <c r="B1" t="str">
-        <v>goodbye</v>
+        <v>TeamNum</v>
       </c>
       <c r="C1" t="str">
-        <v>NO</v>
+        <v>climb</v>
       </c>
       <c r="D1" t="str">
-        <v>boooooo</v>
+        <v>throw</v>
+      </c>
+      <c r="E1" t="str">
+        <v>additionalNotes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1</v>
+        <v>324</v>
       </c>
       <c r="B2" t="str">
-        <v>2</v>
+        <v>1234</v>
       </c>
       <c r="C2" t="str">
-        <v>3</v>
+        <v>No</v>
       </c>
       <c r="D2" t="str">
-        <v>4</v>
+        <v>Yes</v>
+      </c>
+      <c r="E2" t="str">
+        <v>49iulfkhdjkhlksajd23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="B3" t="str">
-        <v>2</v>
+        <v>2341234</v>
       </c>
       <c r="C3" t="str">
-        <v>3</v>
+        <v>No</v>
       </c>
       <c r="D3" t="str">
-        <v>4</v>
+        <v>Yes</v>
+      </c>
+      <c r="E3" t="str">
+        <v>sd32wedaslr2h14lhrkjasgkh</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>231</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3214</v>
+      </c>
+      <c r="C4" t="str">
+        <v>No</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E4" t="str">
+        <v>hdfkjhlskdf</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>53</v>
+      </c>
+      <c r="B5" t="str">
+        <v>4123</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D5" t="str">
+        <v>No</v>
+      </c>
+      <c r="E5" t="str">
+        <v>421341234</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>